<commit_message>
Schreiben in Templates als Funtion, examples aktualisiert
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -29,55 +29,55 @@
     <t xml:space="preserve">MainInput</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/5MW_Land_DLL_WTurb.fst</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/5MW_Land_DLL_WTurb.fst</t>
   </si>
   <si>
     <t xml:space="preserve">ElastoDyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
   </si>
   <si>
     <t xml:space="preserve">ServoDyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Aerodyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Inflowind</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Turbsim</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/wind/TurbSim.inp</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/wind/TurbSim.inp</t>
   </si>
   <si>
     <t xml:space="preserve">IECWind</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/wind/IEC_template.IPT</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/wind/IEC_template.IPT</t>
   </si>
   <si>
     <t xml:space="preserve">Simulation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim</t>
   </si>
   <si>
     <t xml:space="preserve">Wind directory</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/wind</t>
+    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/wind</t>
   </si>
   <si>
     <t xml:space="preserve">DLC Group</t>
@@ -137,45 +137,42 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[12 14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;[10 20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;10:10:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;a&gt;[-8:8:8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEC:ECD+R</t>
   </si>
   <si>
     <t xml:space="preserve">8</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1p1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[12 14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;[10 20]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;10:10:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;a&gt;[-8:8:8]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1p2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IEC:ECD+R</t>
-  </si>
-  <si>
     <t xml:space="preserve">50</t>
   </si>
   <si>
@@ -186,12 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve">ETM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
   </si>
 </sst>
 </file>
@@ -425,7 +416,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,7 +439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -534,7 +525,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -546,7 +537,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="18.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="1.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.55"/>
@@ -615,104 +606,89 @@
       <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="L3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bearbeitung d. Kommentare aus 2. code review
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -29,55 +29,199 @@
     <t xml:space="preserve">MainInput</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/5MW_Land_DLL_WTurb.fst</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sim/5MW_Land_DLL_WTurb.fst</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ElastoDyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ServoDyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Aerodyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Inflowind</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Turbsim</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/wind/TurbSim.inp</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wind/TurbSim.inp</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">IECWind</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/wind/IEC_template.IPT</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wind/IEC_template.IPT</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Simulation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/sim</t>
+    <t xml:space="preserve">../examples/sim</t>
   </si>
   <si>
     <t xml:space="preserve">Wind directory</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_sim/wind</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">../examples/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Sans Serif"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wind</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">DLC Group</t>
@@ -183,9 +327,6 @@
   </si>
   <si>
     <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ;</t>
   </si>
 </sst>
 </file>
@@ -196,7 +337,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -226,6 +367,12 @@
       <name val="CMU Sans Serif"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="CMU Sans Serif"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -311,11 +458,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,8 +565,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B18:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -434,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -450,15 +597,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -466,7 +613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -474,7 +621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -482,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -501,11 +648,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -525,10 +672,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="B18:B19 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -698,11 +845,6 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
separated template files from generated files; reduces example simulation time to 10s for faster validation; added function to copy all required files to target directory; changed IEC_template.IPT for new iecwind version with support for S class turbulence
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,199 +29,55 @@
     <t xml:space="preserve">MainInput</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">sim/5MW_Land_DLL_WTurb.fst</t>
-    </r>
+    <t xml:space="preserve">../examples/templates/sim/5MW_Land_DLL_WTurb.fst</t>
   </si>
   <si>
     <t xml:space="preserve">ElastoDyn</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
-    </r>
+    <t xml:space="preserve">../examples/templates/sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
   </si>
   <si>
     <t xml:space="preserve">ServoDyn</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
-    </r>
+    <t xml:space="preserve">../examples/templates/sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Aerodyn</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
-    </r>
+    <t xml:space="preserve">../examples/templates/sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Inflowind</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
-    </r>
+    <t xml:space="preserve">../examples/templates/sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Turbsim</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">wind/TurbSim.inp</t>
-    </r>
+    <t xml:space="preserve">../examples/templates/wind/TurbSim.inp</t>
   </si>
   <si>
     <t xml:space="preserve">IECWind</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">wind/IEC_template.IPT</t>
-    </r>
+    <t xml:space="preserve">../examples/templates/wind/IEC_template.IPT</t>
   </si>
   <si>
     <t xml:space="preserve">Simulation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">../examples/sim</t>
+    <t xml:space="preserve">../examples/generated/sim</t>
   </si>
   <si>
     <t xml:space="preserve">Wind directory</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">../examples/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CMU Sans Serif"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">wind</t>
-    </r>
+    <t xml:space="preserve">../examples/generated/wind</t>
   </si>
   <si>
     <t xml:space="preserve">DLC Group</t>
@@ -281,7 +137,7 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">60</t>
+    <t xml:space="preserve">10</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
@@ -337,7 +193,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -367,12 +223,6 @@
       <name val="CMU Sans Serif"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="CMU Sans Serif"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -458,11 +308,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,11 +415,11 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B18:B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.22"/>
@@ -581,7 +431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -589,7 +439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -597,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -605,7 +455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -613,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -621,7 +471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -629,7 +479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -648,7 +498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -674,11 +524,11 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="B18:B19 B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.58"/>
@@ -688,7 +538,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="18.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="1.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="1.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.55"/>

</xml_diff>

<commit_message>
paths in Excel config are now relative to Excel file; ampows adds itself to path
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -71,13 +71,13 @@
     <t xml:space="preserve">Simulation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">../examples/generated/sim</t>
+    <t xml:space="preserve">./generated/sim</t>
   </si>
   <si>
     <t xml:space="preserve">Wind directory</t>
   </si>
   <si>
-    <t xml:space="preserve">../examples/generated/wind</t>
+    <t xml:space="preserve">./generated/wind</t>
   </si>
   <si>
     <t xml:space="preserve">DLC Group</t>
@@ -415,8 +415,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -524,7 +524,7 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
enabled generation of multiple IEC wind conditions per DLC line; added cut-in, cut-out and rated wind speed as xls configuration parameters; fixed handling of wind class and turbulence class; added automatic calculation of rotor diameter and tower height
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -80,6 +80,24 @@
     <t xml:space="preserve">./generated/wind</t>
   </si>
   <si>
+    <t xml:space="preserve">Cut-in wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cut-out wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
     <t xml:space="preserve">DLC Group</t>
   </si>
   <si>
@@ -89,6 +107,9 @@
     <t xml:space="preserve">Wind-Speed</t>
   </si>
   <si>
+    <t xml:space="preserve">Wind-Class</t>
+  </si>
+  <si>
     <t xml:space="preserve">Turb-Class</t>
   </si>
   <si>
@@ -137,6 +158,9 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
@@ -167,7 +191,7 @@
     <t xml:space="preserve">1p4</t>
   </si>
   <si>
-    <t xml:space="preserve">IEC:ECD+R</t>
+    <t xml:space="preserve">IEC:ECD+R:ECD+R+2.0:ECD+R-2.0</t>
   </si>
   <si>
     <t xml:space="preserve">8</t>
@@ -413,10 +437,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -504,6 +528,30 @@
       </c>
       <c r="B11" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -522,10 +570,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -533,166 +581,181 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="18.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="1.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="1.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="11.55"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="L3" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="H4" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>38</v>
+        <v>57</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added generation of impulse and ramp wind; added copyright to all files
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -207,6 +207,33 @@
   </si>
   <si>
     <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMP:+1/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[v_r-2 v_r v_r+2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ramp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMP:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1100</t>
   </si>
 </sst>
 </file>
@@ -440,7 +467,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -570,10 +597,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -758,6 +785,52 @@
         <v>61</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added possibility to use pregenerated bts files; added tool to make rotor coherent wind file from spacially turbulent bts file
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -173,19 +173,16 @@
     <t xml:space="preserve">ETM</t>
   </si>
   <si>
-    <t xml:space="preserve">[12 14]</t>
+    <t xml:space="preserve">[10 12]</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;[10 20]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;10:10:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;a&gt;[-8:8:8]</t>
+    <t xml:space="preserve">&lt;b&gt;[5 7]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;a&gt;[-2:2:2]</t>
   </si>
   <si>
     <t xml:space="preserve">1p4</t>
@@ -234,6 +231,12 @@
   </si>
   <si>
     <t xml:space="preserve">1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTS:NTM_URef-%d_turbsim_coh</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="N3 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,10 +600,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -724,21 +727,21 @@
         <v>52</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="P3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>44</v>
@@ -747,7 +750,7 @@
         <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>47</v>
@@ -756,15 +759,15 @@
         <v>46</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>44</v>
@@ -773,7 +776,7 @@
         <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>47</v>
@@ -782,53 +785,64 @@
         <v>46</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>67</v>
+      <c r="B8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added possibility to configure the output sensors via an xlsx list that is referenced in the config sheet of the main config xlsx file
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OutSensors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./OutListParameters.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">DLC Group</t>
@@ -467,10 +473,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="N3 B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -582,6 +588,14 @@
       </c>
       <c r="B15" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +616,7 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -627,222 +641,222 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed that premade bts files need to be configured with a known duration
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -475,7 +475,7 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -616,8 +616,8 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -858,6 +858,9 @@
       <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added possibility to specify OpenFAST and turbsim executable file path in config sheet
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t xml:space="preserve">./OutListParameters.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenFAST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turbsim</t>
   </si>
   <si>
     <t xml:space="preserve">DLC Group</t>
@@ -473,10 +482,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -596,6 +605,22 @@
       </c>
       <c r="B17" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +641,7 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -641,225 +666,225 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added processing of sub structure files; the sub-files in the config-xslx may now be left empty; wind related entries may be left empty, if no wind files need to be generated; usage of pre-computed Bladed-wnd-files is now supported; the file names of pre-computed bts and wnd files may now contain Uref (substitute by %1) and randseed (substitute by %2); group variations are named by the group name; initial conditions may be set via wind0, theta0, omega0 and tow_fa0 depending on Uref
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">coh</t>
   </si>
   <si>
-    <t xml:space="preserve">BTS:NTM_URef-%d_turbsim_coh</t>
+    <t xml:space="preserve">BTS:NTM_URef-%1$d_turbsim_coh</t>
   </si>
 </sst>
 </file>
@@ -484,13 +484,13 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.55"/>
   </cols>
@@ -625,8 +625,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -641,8 +641,8 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,8 +889,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
fixed wrong processing order of turbsim after inflowwind; added possibility to variation mark group name with an ! to indicate its value should be used to identify group elements
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -113,6 +113,30 @@
     <t xml:space="preserve">turbsim</t>
   </si>
   <si>
+    <t xml:space="preserve">wind0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1  25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0  30]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omega0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[4 12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tow_fa0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0 0.6]</t>
+  </si>
+  <si>
     <t xml:space="preserve">DLC Group</t>
   </si>
   <si>
@@ -161,13 +185,19 @@
     <t xml:space="preserve">YawNeut</t>
   </si>
   <si>
+    <t xml:space="preserve">RotSpeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTDspFA</t>
+  </si>
+  <si>
     <t xml:space="preserve">1p1</t>
   </si>
   <si>
     <t xml:space="preserve">NTM</t>
   </si>
   <si>
-    <t xml:space="preserve">[10 20]</t>
+    <t xml:space="preserve">&lt;URef&gt;repmat(10:11, 1, 3)</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -179,79 +209,91 @@
     <t xml:space="preserve">10</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;!URef&gt;reshape((10:11)'*10+(0:2), 1, [])</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> omega0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tow_fa0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;[5 7]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;a&gt;[-2:2:2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEC:ECD+R:ECD+R+2.0:ECD+R-2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">1p3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETM</t>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEC:EWSH+12.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMP:+1/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[v_r-2 v_r v_r+2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ramp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMP:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prewind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTS:../wind/URef_%1$02d_Seed_%1$02d%2$02d </t>
   </si>
   <si>
     <t xml:space="preserve">[10 12]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;[5 7]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;a&gt;[-2:2:2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1p4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IEC:ECD+R:ECD+R+2.0:ECD+R-2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1p5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IEC:EWSH+12.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impulse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMP:+1/5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[v_r-2 v_r v_r+2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ramp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMP:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BTS:NTM_URef-%1$d_turbsim_coh</t>
   </si>
 </sst>
 </file>
@@ -262,7 +304,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -300,6 +342,12 @@
       <name val="CMU Sans Serif"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="CMU Sans Serif"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -364,7 +412,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -402,6 +450,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -482,15 +534,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.55"/>
   </cols>
@@ -621,6 +673,38 @@
       </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -639,10 +723,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -661,230 +745,273 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="11.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="17" style="1" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>45</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>89</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>90</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>51</v>
+        <v>61</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>